<commit_message>
changes at the ui-diagramms
</commit_message>
<xml_diff>
--- a/UserStory1_User/Konzept_Phase1/Zeitplanung/Gantt-Diagramm.xlsx
+++ b/UserStory1_User/Konzept_Phase1/Zeitplanung/Gantt-Diagramm.xlsx
@@ -902,6 +902,30 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -920,34 +944,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1001,7 +1001,7 @@
         <xdr:cNvPr id="29" name="Rechteck 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1071,7 +1071,7 @@
         <xdr:cNvPr id="81" name="Rechteck 80">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000051000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000051000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1138,7 +1138,7 @@
         <xdr:cNvPr id="82" name="Rechteck 81">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000052000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000052000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1211,7 +1211,7 @@
         <xdr:cNvPr id="85" name="Rechteck 84">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000055000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1283,7 +1283,7 @@
         <xdr:cNvPr id="23" name="Raute 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1351,7 +1351,7 @@
         <xdr:cNvPr id="21" name="Rechteck 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000015000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1421,7 +1421,7 @@
         <xdr:cNvPr id="25" name="Raute 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1489,7 +1489,7 @@
         <xdr:cNvPr id="26" name="Raute 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1557,7 +1557,7 @@
         <xdr:cNvPr id="30" name="Raute 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1625,7 +1625,7 @@
         <xdr:cNvPr id="12" name="Rechteck 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1698,7 +1698,7 @@
         <xdr:cNvPr id="13" name="Raute 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1766,7 +1766,7 @@
         <xdr:cNvPr id="15" name="Raute 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2156,8 +2156,8 @@
   </sheetPr>
   <dimension ref="A1:FJ62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX16" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="CT21" sqref="CT21"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2187,174 +2187,174 @@
       <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="92" t="s">
+      <c r="F1" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="86"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="86"/>
-      <c r="U1" s="93"/>
-      <c r="V1" s="86" t="s">
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="85"/>
+      <c r="V1" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="86"/>
-      <c r="X1" s="86"/>
-      <c r="Y1" s="86"/>
-      <c r="Z1" s="86"/>
-      <c r="AA1" s="86"/>
-      <c r="AB1" s="86"/>
-      <c r="AC1" s="86"/>
-      <c r="AD1" s="86"/>
-      <c r="AE1" s="86"/>
-      <c r="AF1" s="86"/>
-      <c r="AG1" s="86"/>
-      <c r="AH1" s="86"/>
-      <c r="AI1" s="86"/>
-      <c r="AJ1" s="86"/>
-      <c r="AK1" s="86"/>
-      <c r="AL1" s="86"/>
-      <c r="AM1" s="86"/>
-      <c r="AN1" s="86"/>
-      <c r="AO1" s="86"/>
-      <c r="AP1" s="86"/>
-      <c r="AQ1" s="86"/>
-      <c r="AR1" s="86"/>
-      <c r="AS1" s="86"/>
-      <c r="AT1" s="86"/>
-      <c r="AU1" s="86"/>
-      <c r="AV1" s="86"/>
-      <c r="AW1" s="86"/>
-      <c r="AX1" s="86"/>
-      <c r="AY1" s="86"/>
-      <c r="AZ1" s="86"/>
-      <c r="BA1" s="91"/>
-      <c r="BB1" s="94" t="s">
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
+      <c r="AG1" s="84"/>
+      <c r="AH1" s="84"/>
+      <c r="AI1" s="84"/>
+      <c r="AJ1" s="84"/>
+      <c r="AK1" s="84"/>
+      <c r="AL1" s="84"/>
+      <c r="AM1" s="84"/>
+      <c r="AN1" s="84"/>
+      <c r="AO1" s="84"/>
+      <c r="AP1" s="84"/>
+      <c r="AQ1" s="84"/>
+      <c r="AR1" s="84"/>
+      <c r="AS1" s="84"/>
+      <c r="AT1" s="84"/>
+      <c r="AU1" s="84"/>
+      <c r="AV1" s="84"/>
+      <c r="AW1" s="84"/>
+      <c r="AX1" s="84"/>
+      <c r="AY1" s="84"/>
+      <c r="AZ1" s="84"/>
+      <c r="BA1" s="95"/>
+      <c r="BB1" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="BC1" s="86"/>
-      <c r="BD1" s="86"/>
-      <c r="BE1" s="86"/>
-      <c r="BF1" s="86"/>
-      <c r="BG1" s="86"/>
-      <c r="BH1" s="86"/>
-      <c r="BI1" s="86"/>
-      <c r="BJ1" s="86"/>
-      <c r="BK1" s="86"/>
-      <c r="BL1" s="86"/>
-      <c r="BM1" s="86"/>
-      <c r="BN1" s="86"/>
-      <c r="BO1" s="86"/>
-      <c r="BP1" s="86"/>
-      <c r="BQ1" s="86"/>
-      <c r="BR1" s="86"/>
-      <c r="BS1" s="86"/>
-      <c r="BT1" s="86"/>
-      <c r="BU1" s="86"/>
-      <c r="BV1" s="86"/>
-      <c r="BW1" s="86"/>
-      <c r="BX1" s="86"/>
-      <c r="BY1" s="86"/>
-      <c r="BZ1" s="86"/>
-      <c r="CA1" s="86"/>
-      <c r="CB1" s="86"/>
-      <c r="CC1" s="86"/>
-      <c r="CD1" s="86"/>
-      <c r="CE1" s="86"/>
-      <c r="CF1" s="86"/>
-      <c r="CG1" s="86"/>
-      <c r="CH1" s="86"/>
-      <c r="CI1" s="86"/>
-      <c r="CJ1" s="86"/>
-      <c r="CK1" s="86"/>
-      <c r="CL1" s="86"/>
-      <c r="CM1" s="86"/>
-      <c r="CN1" s="86"/>
-      <c r="CO1" s="86"/>
-      <c r="CP1" s="86"/>
-      <c r="CQ1" s="86"/>
-      <c r="CR1" s="86"/>
-      <c r="CS1" s="86"/>
-      <c r="CT1" s="86"/>
-      <c r="CU1" s="86"/>
-      <c r="CV1" s="86"/>
-      <c r="CW1" s="86"/>
-      <c r="CX1" s="86"/>
-      <c r="CY1" s="86"/>
-      <c r="CZ1" s="86"/>
-      <c r="DA1" s="86"/>
-      <c r="DB1" s="86"/>
-      <c r="DC1" s="86"/>
-      <c r="DD1" s="86"/>
-      <c r="DE1" s="86"/>
-      <c r="DF1" s="86"/>
-      <c r="DG1" s="86"/>
-      <c r="DH1" s="86"/>
-      <c r="DI1" s="86"/>
-      <c r="DJ1" s="86"/>
-      <c r="DK1" s="86"/>
-      <c r="DL1" s="86"/>
-      <c r="DM1" s="95"/>
-      <c r="DN1" s="86" t="s">
+      <c r="BC1" s="84"/>
+      <c r="BD1" s="84"/>
+      <c r="BE1" s="84"/>
+      <c r="BF1" s="84"/>
+      <c r="BG1" s="84"/>
+      <c r="BH1" s="84"/>
+      <c r="BI1" s="84"/>
+      <c r="BJ1" s="84"/>
+      <c r="BK1" s="84"/>
+      <c r="BL1" s="84"/>
+      <c r="BM1" s="84"/>
+      <c r="BN1" s="84"/>
+      <c r="BO1" s="84"/>
+      <c r="BP1" s="84"/>
+      <c r="BQ1" s="84"/>
+      <c r="BR1" s="84"/>
+      <c r="BS1" s="84"/>
+      <c r="BT1" s="84"/>
+      <c r="BU1" s="84"/>
+      <c r="BV1" s="84"/>
+      <c r="BW1" s="84"/>
+      <c r="BX1" s="84"/>
+      <c r="BY1" s="84"/>
+      <c r="BZ1" s="84"/>
+      <c r="CA1" s="84"/>
+      <c r="CB1" s="84"/>
+      <c r="CC1" s="84"/>
+      <c r="CD1" s="84"/>
+      <c r="CE1" s="84"/>
+      <c r="CF1" s="84"/>
+      <c r="CG1" s="84"/>
+      <c r="CH1" s="84"/>
+      <c r="CI1" s="84"/>
+      <c r="CJ1" s="84"/>
+      <c r="CK1" s="84"/>
+      <c r="CL1" s="84"/>
+      <c r="CM1" s="84"/>
+      <c r="CN1" s="84"/>
+      <c r="CO1" s="84"/>
+      <c r="CP1" s="84"/>
+      <c r="CQ1" s="84"/>
+      <c r="CR1" s="84"/>
+      <c r="CS1" s="84"/>
+      <c r="CT1" s="84"/>
+      <c r="CU1" s="84"/>
+      <c r="CV1" s="84"/>
+      <c r="CW1" s="84"/>
+      <c r="CX1" s="84"/>
+      <c r="CY1" s="84"/>
+      <c r="CZ1" s="84"/>
+      <c r="DA1" s="84"/>
+      <c r="DB1" s="84"/>
+      <c r="DC1" s="84"/>
+      <c r="DD1" s="84"/>
+      <c r="DE1" s="84"/>
+      <c r="DF1" s="84"/>
+      <c r="DG1" s="84"/>
+      <c r="DH1" s="84"/>
+      <c r="DI1" s="84"/>
+      <c r="DJ1" s="84"/>
+      <c r="DK1" s="84"/>
+      <c r="DL1" s="84"/>
+      <c r="DM1" s="87"/>
+      <c r="DN1" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="DO1" s="86"/>
-      <c r="DP1" s="86"/>
-      <c r="DQ1" s="86"/>
-      <c r="DR1" s="86"/>
-      <c r="DS1" s="86"/>
-      <c r="DT1" s="86"/>
-      <c r="DU1" s="86"/>
-      <c r="DV1" s="86"/>
-      <c r="DW1" s="86"/>
-      <c r="DX1" s="86"/>
-      <c r="DY1" s="86"/>
-      <c r="DZ1" s="86"/>
-      <c r="EA1" s="86"/>
-      <c r="EB1" s="86"/>
-      <c r="EC1" s="86"/>
-      <c r="ED1" s="86"/>
-      <c r="EE1" s="86"/>
-      <c r="EF1" s="86"/>
-      <c r="EG1" s="86"/>
-      <c r="EH1" s="86"/>
-      <c r="EI1" s="86"/>
-      <c r="EJ1" s="86"/>
-      <c r="EK1" s="86"/>
-      <c r="EL1" s="86"/>
-      <c r="EM1" s="86"/>
-      <c r="EN1" s="86"/>
-      <c r="EO1" s="86"/>
-      <c r="EP1" s="86"/>
-      <c r="EQ1" s="86"/>
-      <c r="ER1" s="86"/>
-      <c r="ES1" s="86"/>
-      <c r="ET1" s="86"/>
-      <c r="EU1" s="86"/>
-      <c r="EV1" s="86"/>
-      <c r="EW1" s="86"/>
-      <c r="EX1" s="86"/>
-      <c r="EY1" s="86"/>
-      <c r="EZ1" s="86"/>
-      <c r="FA1" s="86"/>
-      <c r="FB1" s="86"/>
-      <c r="FC1" s="86"/>
-      <c r="FD1" s="86"/>
-      <c r="FE1" s="86"/>
-      <c r="FF1" s="86"/>
-      <c r="FG1" s="86"/>
-      <c r="FH1" s="86"/>
-      <c r="FI1" s="87"/>
+      <c r="DO1" s="84"/>
+      <c r="DP1" s="84"/>
+      <c r="DQ1" s="84"/>
+      <c r="DR1" s="84"/>
+      <c r="DS1" s="84"/>
+      <c r="DT1" s="84"/>
+      <c r="DU1" s="84"/>
+      <c r="DV1" s="84"/>
+      <c r="DW1" s="84"/>
+      <c r="DX1" s="84"/>
+      <c r="DY1" s="84"/>
+      <c r="DZ1" s="84"/>
+      <c r="EA1" s="84"/>
+      <c r="EB1" s="84"/>
+      <c r="EC1" s="84"/>
+      <c r="ED1" s="84"/>
+      <c r="EE1" s="84"/>
+      <c r="EF1" s="84"/>
+      <c r="EG1" s="84"/>
+      <c r="EH1" s="84"/>
+      <c r="EI1" s="84"/>
+      <c r="EJ1" s="84"/>
+      <c r="EK1" s="84"/>
+      <c r="EL1" s="84"/>
+      <c r="EM1" s="84"/>
+      <c r="EN1" s="84"/>
+      <c r="EO1" s="84"/>
+      <c r="EP1" s="84"/>
+      <c r="EQ1" s="84"/>
+      <c r="ER1" s="84"/>
+      <c r="ES1" s="84"/>
+      <c r="ET1" s="84"/>
+      <c r="EU1" s="84"/>
+      <c r="EV1" s="84"/>
+      <c r="EW1" s="84"/>
+      <c r="EX1" s="84"/>
+      <c r="EY1" s="84"/>
+      <c r="EZ1" s="84"/>
+      <c r="FA1" s="84"/>
+      <c r="FB1" s="84"/>
+      <c r="FC1" s="84"/>
+      <c r="FD1" s="84"/>
+      <c r="FE1" s="84"/>
+      <c r="FF1" s="84"/>
+      <c r="FG1" s="84"/>
+      <c r="FH1" s="84"/>
+      <c r="FI1" s="94"/>
     </row>
     <row r="2" spans="1:165" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -2366,186 +2366,186 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="88">
+      <c r="F2" s="80">
         <v>42901</v>
       </c>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="89"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="88">
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="82"/>
+      <c r="V2" s="80">
         <v>42907</v>
       </c>
-      <c r="W2" s="89"/>
-      <c r="X2" s="89"/>
-      <c r="Y2" s="89"/>
-      <c r="Z2" s="89"/>
-      <c r="AA2" s="89"/>
-      <c r="AB2" s="89"/>
-      <c r="AC2" s="89"/>
-      <c r="AD2" s="89"/>
-      <c r="AE2" s="89"/>
-      <c r="AF2" s="89"/>
-      <c r="AG2" s="89"/>
-      <c r="AH2" s="89"/>
-      <c r="AI2" s="89"/>
-      <c r="AJ2" s="89"/>
-      <c r="AK2" s="90"/>
-      <c r="AL2" s="88">
+      <c r="W2" s="81"/>
+      <c r="X2" s="81"/>
+      <c r="Y2" s="81"/>
+      <c r="Z2" s="81"/>
+      <c r="AA2" s="81"/>
+      <c r="AB2" s="81"/>
+      <c r="AC2" s="81"/>
+      <c r="AD2" s="81"/>
+      <c r="AE2" s="81"/>
+      <c r="AF2" s="81"/>
+      <c r="AG2" s="81"/>
+      <c r="AH2" s="81"/>
+      <c r="AI2" s="81"/>
+      <c r="AJ2" s="81"/>
+      <c r="AK2" s="82"/>
+      <c r="AL2" s="80">
         <v>42908</v>
       </c>
-      <c r="AM2" s="89"/>
-      <c r="AN2" s="89"/>
-      <c r="AO2" s="89"/>
-      <c r="AP2" s="89"/>
-      <c r="AQ2" s="89"/>
-      <c r="AR2" s="89"/>
-      <c r="AS2" s="89"/>
-      <c r="AT2" s="89"/>
-      <c r="AU2" s="89"/>
-      <c r="AV2" s="89"/>
-      <c r="AW2" s="89"/>
-      <c r="AX2" s="89"/>
-      <c r="AY2" s="89"/>
-      <c r="AZ2" s="89"/>
-      <c r="BA2" s="90"/>
-      <c r="BB2" s="88">
+      <c r="AM2" s="81"/>
+      <c r="AN2" s="81"/>
+      <c r="AO2" s="81"/>
+      <c r="AP2" s="81"/>
+      <c r="AQ2" s="81"/>
+      <c r="AR2" s="81"/>
+      <c r="AS2" s="81"/>
+      <c r="AT2" s="81"/>
+      <c r="AU2" s="81"/>
+      <c r="AV2" s="81"/>
+      <c r="AW2" s="81"/>
+      <c r="AX2" s="81"/>
+      <c r="AY2" s="81"/>
+      <c r="AZ2" s="81"/>
+      <c r="BA2" s="82"/>
+      <c r="BB2" s="80">
         <v>42913</v>
       </c>
-      <c r="BC2" s="89"/>
-      <c r="BD2" s="89"/>
-      <c r="BE2" s="89"/>
-      <c r="BF2" s="89"/>
-      <c r="BG2" s="89"/>
-      <c r="BH2" s="89"/>
-      <c r="BI2" s="89"/>
-      <c r="BJ2" s="89"/>
-      <c r="BK2" s="89"/>
-      <c r="BL2" s="89"/>
-      <c r="BM2" s="89"/>
-      <c r="BN2" s="89"/>
-      <c r="BO2" s="89"/>
-      <c r="BP2" s="89"/>
-      <c r="BQ2" s="90"/>
-      <c r="BR2" s="88">
+      <c r="BC2" s="81"/>
+      <c r="BD2" s="81"/>
+      <c r="BE2" s="81"/>
+      <c r="BF2" s="81"/>
+      <c r="BG2" s="81"/>
+      <c r="BH2" s="81"/>
+      <c r="BI2" s="81"/>
+      <c r="BJ2" s="81"/>
+      <c r="BK2" s="81"/>
+      <c r="BL2" s="81"/>
+      <c r="BM2" s="81"/>
+      <c r="BN2" s="81"/>
+      <c r="BO2" s="81"/>
+      <c r="BP2" s="81"/>
+      <c r="BQ2" s="82"/>
+      <c r="BR2" s="80">
         <v>42914</v>
       </c>
-      <c r="BS2" s="89"/>
-      <c r="BT2" s="89"/>
-      <c r="BU2" s="89"/>
-      <c r="BV2" s="89"/>
-      <c r="BW2" s="89"/>
-      <c r="BX2" s="89"/>
-      <c r="BY2" s="89"/>
-      <c r="BZ2" s="89"/>
-      <c r="CA2" s="89"/>
-      <c r="CB2" s="89"/>
-      <c r="CC2" s="89"/>
-      <c r="CD2" s="89"/>
-      <c r="CE2" s="89"/>
-      <c r="CF2" s="89"/>
-      <c r="CG2" s="90"/>
-      <c r="CH2" s="88">
+      <c r="BS2" s="81"/>
+      <c r="BT2" s="81"/>
+      <c r="BU2" s="81"/>
+      <c r="BV2" s="81"/>
+      <c r="BW2" s="81"/>
+      <c r="BX2" s="81"/>
+      <c r="BY2" s="81"/>
+      <c r="BZ2" s="81"/>
+      <c r="CA2" s="81"/>
+      <c r="CB2" s="81"/>
+      <c r="CC2" s="81"/>
+      <c r="CD2" s="81"/>
+      <c r="CE2" s="81"/>
+      <c r="CF2" s="81"/>
+      <c r="CG2" s="82"/>
+      <c r="CH2" s="80">
         <v>42915</v>
       </c>
-      <c r="CI2" s="89"/>
-      <c r="CJ2" s="89"/>
-      <c r="CK2" s="89"/>
-      <c r="CL2" s="89"/>
-      <c r="CM2" s="89"/>
-      <c r="CN2" s="89"/>
-      <c r="CO2" s="89"/>
-      <c r="CP2" s="89"/>
-      <c r="CQ2" s="89"/>
-      <c r="CR2" s="89"/>
-      <c r="CS2" s="89"/>
-      <c r="CT2" s="89"/>
-      <c r="CU2" s="89"/>
-      <c r="CV2" s="89"/>
-      <c r="CW2" s="90"/>
-      <c r="CX2" s="88">
+      <c r="CI2" s="81"/>
+      <c r="CJ2" s="81"/>
+      <c r="CK2" s="81"/>
+      <c r="CL2" s="81"/>
+      <c r="CM2" s="81"/>
+      <c r="CN2" s="81"/>
+      <c r="CO2" s="81"/>
+      <c r="CP2" s="81"/>
+      <c r="CQ2" s="81"/>
+      <c r="CR2" s="81"/>
+      <c r="CS2" s="81"/>
+      <c r="CT2" s="81"/>
+      <c r="CU2" s="81"/>
+      <c r="CV2" s="81"/>
+      <c r="CW2" s="82"/>
+      <c r="CX2" s="80">
         <v>42916</v>
       </c>
-      <c r="CY2" s="89"/>
-      <c r="CZ2" s="89"/>
-      <c r="DA2" s="89"/>
-      <c r="DB2" s="89"/>
-      <c r="DC2" s="89"/>
-      <c r="DD2" s="89"/>
-      <c r="DE2" s="89"/>
-      <c r="DF2" s="89"/>
-      <c r="DG2" s="89"/>
-      <c r="DH2" s="89"/>
-      <c r="DI2" s="89"/>
-      <c r="DJ2" s="89"/>
-      <c r="DK2" s="89"/>
-      <c r="DL2" s="89"/>
-      <c r="DM2" s="90"/>
-      <c r="DN2" s="88">
+      <c r="CY2" s="81"/>
+      <c r="CZ2" s="81"/>
+      <c r="DA2" s="81"/>
+      <c r="DB2" s="81"/>
+      <c r="DC2" s="81"/>
+      <c r="DD2" s="81"/>
+      <c r="DE2" s="81"/>
+      <c r="DF2" s="81"/>
+      <c r="DG2" s="81"/>
+      <c r="DH2" s="81"/>
+      <c r="DI2" s="81"/>
+      <c r="DJ2" s="81"/>
+      <c r="DK2" s="81"/>
+      <c r="DL2" s="81"/>
+      <c r="DM2" s="82"/>
+      <c r="DN2" s="80">
         <v>42921</v>
       </c>
-      <c r="DO2" s="89"/>
-      <c r="DP2" s="89"/>
-      <c r="DQ2" s="89"/>
-      <c r="DR2" s="89"/>
-      <c r="DS2" s="89"/>
-      <c r="DT2" s="89"/>
-      <c r="DU2" s="89"/>
-      <c r="DV2" s="89"/>
-      <c r="DW2" s="89"/>
-      <c r="DX2" s="89"/>
-      <c r="DY2" s="89"/>
-      <c r="DZ2" s="89"/>
-      <c r="EA2" s="89"/>
-      <c r="EB2" s="89"/>
-      <c r="EC2" s="90"/>
-      <c r="ED2" s="88">
+      <c r="DO2" s="81"/>
+      <c r="DP2" s="81"/>
+      <c r="DQ2" s="81"/>
+      <c r="DR2" s="81"/>
+      <c r="DS2" s="81"/>
+      <c r="DT2" s="81"/>
+      <c r="DU2" s="81"/>
+      <c r="DV2" s="81"/>
+      <c r="DW2" s="81"/>
+      <c r="DX2" s="81"/>
+      <c r="DY2" s="81"/>
+      <c r="DZ2" s="81"/>
+      <c r="EA2" s="81"/>
+      <c r="EB2" s="81"/>
+      <c r="EC2" s="82"/>
+      <c r="ED2" s="80">
         <v>42953</v>
       </c>
-      <c r="EE2" s="89"/>
-      <c r="EF2" s="89"/>
-      <c r="EG2" s="89"/>
-      <c r="EH2" s="89"/>
-      <c r="EI2" s="89"/>
-      <c r="EJ2" s="89"/>
-      <c r="EK2" s="89"/>
-      <c r="EL2" s="89"/>
-      <c r="EM2" s="89"/>
-      <c r="EN2" s="89"/>
-      <c r="EO2" s="89"/>
-      <c r="EP2" s="89"/>
-      <c r="EQ2" s="89"/>
-      <c r="ER2" s="89"/>
-      <c r="ES2" s="90"/>
-      <c r="ET2" s="88">
+      <c r="EE2" s="81"/>
+      <c r="EF2" s="81"/>
+      <c r="EG2" s="81"/>
+      <c r="EH2" s="81"/>
+      <c r="EI2" s="81"/>
+      <c r="EJ2" s="81"/>
+      <c r="EK2" s="81"/>
+      <c r="EL2" s="81"/>
+      <c r="EM2" s="81"/>
+      <c r="EN2" s="81"/>
+      <c r="EO2" s="81"/>
+      <c r="EP2" s="81"/>
+      <c r="EQ2" s="81"/>
+      <c r="ER2" s="81"/>
+      <c r="ES2" s="82"/>
+      <c r="ET2" s="80">
         <v>42923</v>
       </c>
-      <c r="EU2" s="89"/>
-      <c r="EV2" s="89"/>
-      <c r="EW2" s="89"/>
-      <c r="EX2" s="89"/>
-      <c r="EY2" s="89"/>
-      <c r="EZ2" s="89"/>
-      <c r="FA2" s="89"/>
-      <c r="FB2" s="89"/>
-      <c r="FC2" s="89"/>
-      <c r="FD2" s="89"/>
-      <c r="FE2" s="89"/>
-      <c r="FF2" s="89"/>
-      <c r="FG2" s="89"/>
-      <c r="FH2" s="89"/>
-      <c r="FI2" s="90"/>
+      <c r="EU2" s="81"/>
+      <c r="EV2" s="81"/>
+      <c r="EW2" s="81"/>
+      <c r="EX2" s="81"/>
+      <c r="EY2" s="81"/>
+      <c r="EZ2" s="81"/>
+      <c r="FA2" s="81"/>
+      <c r="FB2" s="81"/>
+      <c r="FC2" s="81"/>
+      <c r="FD2" s="81"/>
+      <c r="FE2" s="81"/>
+      <c r="FF2" s="81"/>
+      <c r="FG2" s="81"/>
+      <c r="FH2" s="81"/>
+      <c r="FI2" s="82"/>
     </row>
     <row r="3" spans="1:165" s="47" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="48"/>
@@ -5118,7 +5118,7 @@
       <c r="C18" s="40"/>
       <c r="D18" s="41"/>
       <c r="E18" s="42">
-        <v>15.5</v>
+        <v>22.5</v>
       </c>
       <c r="F18" s="43"/>
       <c r="G18" s="44"/>
@@ -5206,16 +5206,16 @@
       <c r="CK18" s="73"/>
       <c r="CL18" s="73"/>
       <c r="CM18" s="73"/>
-      <c r="CN18" s="44"/>
-      <c r="CO18" s="44"/>
-      <c r="CP18" s="44"/>
-      <c r="CQ18" s="44"/>
-      <c r="CR18" s="44"/>
-      <c r="CS18" s="44"/>
-      <c r="CT18" s="44"/>
-      <c r="CU18" s="44"/>
-      <c r="CV18" s="44"/>
-      <c r="CW18" s="45"/>
+      <c r="CN18" s="73"/>
+      <c r="CO18" s="73"/>
+      <c r="CP18" s="73"/>
+      <c r="CQ18" s="73"/>
+      <c r="CR18" s="73"/>
+      <c r="CS18" s="73"/>
+      <c r="CT18" s="73"/>
+      <c r="CU18" s="73"/>
+      <c r="CV18" s="73"/>
+      <c r="CW18" s="73"/>
       <c r="CX18" s="43"/>
       <c r="CY18" s="44"/>
       <c r="CZ18" s="44"/>
@@ -11371,33 +11371,33 @@
       <c r="B58" t="s">
         <v>49</v>
       </c>
-      <c r="AJ58" s="82" t="s">
+      <c r="AJ58" s="90" t="s">
         <v>55</v>
       </c>
-      <c r="AK58" s="83"/>
-      <c r="AL58" s="83"/>
-      <c r="AM58" s="83"/>
-      <c r="AN58" s="83"/>
-      <c r="AO58" s="83"/>
-      <c r="AP58" s="83"/>
-      <c r="AQ58" s="83"/>
-      <c r="AR58" s="83"/>
-      <c r="AS58" s="83"/>
-      <c r="AT58" s="83"/>
-      <c r="AU58" s="83"/>
-      <c r="AV58" s="83"/>
-      <c r="AW58" s="83"/>
-      <c r="AX58" s="83"/>
-      <c r="AY58" s="83"/>
-      <c r="AZ58" s="83"/>
-      <c r="BA58" s="83"/>
-      <c r="BB58" s="83"/>
-      <c r="BC58" s="83">
+      <c r="AK58" s="91"/>
+      <c r="AL58" s="91"/>
+      <c r="AM58" s="91"/>
+      <c r="AN58" s="91"/>
+      <c r="AO58" s="91"/>
+      <c r="AP58" s="91"/>
+      <c r="AQ58" s="91"/>
+      <c r="AR58" s="91"/>
+      <c r="AS58" s="91"/>
+      <c r="AT58" s="91"/>
+      <c r="AU58" s="91"/>
+      <c r="AV58" s="91"/>
+      <c r="AW58" s="91"/>
+      <c r="AX58" s="91"/>
+      <c r="AY58" s="91"/>
+      <c r="AZ58" s="91"/>
+      <c r="BA58" s="91"/>
+      <c r="BB58" s="91"/>
+      <c r="BC58" s="91">
         <f>SUM(E4,E14,E24,E31,E40,E44,E48,E51)</f>
         <v>20.5</v>
       </c>
-      <c r="BD58" s="83"/>
-      <c r="BE58" s="85"/>
+      <c r="BD58" s="91"/>
+      <c r="BE58" s="93"/>
       <c r="BF58" s="78"/>
       <c r="BG58" s="78"/>
       <c r="BH58" s="78"/>
@@ -11447,33 +11447,33 @@
       <c r="AG59" s="46"/>
       <c r="AH59" s="46"/>
       <c r="AI59" s="46"/>
-      <c r="AJ59" s="80" t="s">
+      <c r="AJ59" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="AK59" s="81"/>
-      <c r="AL59" s="81"/>
-      <c r="AM59" s="81"/>
-      <c r="AN59" s="81"/>
-      <c r="AO59" s="81"/>
-      <c r="AP59" s="81"/>
-      <c r="AQ59" s="81"/>
-      <c r="AR59" s="81"/>
-      <c r="AS59" s="81"/>
-      <c r="AT59" s="81"/>
-      <c r="AU59" s="81"/>
-      <c r="AV59" s="81"/>
-      <c r="AW59" s="81"/>
-      <c r="AX59" s="81"/>
-      <c r="AY59" s="81"/>
-      <c r="AZ59" s="81"/>
-      <c r="BA59" s="81"/>
-      <c r="BB59" s="81"/>
-      <c r="BC59" s="81">
+      <c r="AK59" s="89"/>
+      <c r="AL59" s="89"/>
+      <c r="AM59" s="89"/>
+      <c r="AN59" s="89"/>
+      <c r="AO59" s="89"/>
+      <c r="AP59" s="89"/>
+      <c r="AQ59" s="89"/>
+      <c r="AR59" s="89"/>
+      <c r="AS59" s="89"/>
+      <c r="AT59" s="89"/>
+      <c r="AU59" s="89"/>
+      <c r="AV59" s="89"/>
+      <c r="AW59" s="89"/>
+      <c r="AX59" s="89"/>
+      <c r="AY59" s="89"/>
+      <c r="AZ59" s="89"/>
+      <c r="BA59" s="89"/>
+      <c r="BB59" s="89"/>
+      <c r="BC59" s="89">
         <f>SUM(E6,E8,E10,E12,E16,E18,E20,E22,E26,E33,E37,E42,E46,E50,E53)</f>
-        <v>35</v>
+        <v>42</v>
       </c>
-      <c r="BD59" s="81"/>
-      <c r="BE59" s="84"/>
+      <c r="BD59" s="89"/>
+      <c r="BE59" s="92"/>
       <c r="BF59" s="46"/>
       <c r="BG59" s="46"/>
       <c r="BH59" s="46"/>
@@ -12031,13 +12031,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F2:U2"/>
-    <mergeCell ref="F1:U1"/>
-    <mergeCell ref="V2:AK2"/>
-    <mergeCell ref="AL2:BA2"/>
-    <mergeCell ref="BR2:CG2"/>
-    <mergeCell ref="BB1:DM1"/>
-    <mergeCell ref="BB2:BQ2"/>
     <mergeCell ref="AJ59:BB59"/>
     <mergeCell ref="AJ58:BB58"/>
     <mergeCell ref="BC59:BE59"/>
@@ -12049,6 +12042,13 @@
     <mergeCell ref="V1:BA1"/>
     <mergeCell ref="CH2:CW2"/>
     <mergeCell ref="CX2:DM2"/>
+    <mergeCell ref="F2:U2"/>
+    <mergeCell ref="F1:U1"/>
+    <mergeCell ref="V2:AK2"/>
+    <mergeCell ref="AL2:BA2"/>
+    <mergeCell ref="BR2:CG2"/>
+    <mergeCell ref="BB1:DM1"/>
+    <mergeCell ref="BB2:BQ2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="40" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>